<commit_message>
add recognice of images and click
</commit_message>
<xml_diff>
--- a/framework/test.xlsx
+++ b/framework/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t xml:space="preserve">TestCase</t>
   </si>
@@ -90,10 +90,13 @@
     <t xml:space="preserve">REMOTEDESKTOPNSO</t>
   </si>
   <si>
+    <t xml:space="preserve">REMOTEDESKTOPNSO,NSO</t>
+  </si>
+  <si>
     <t xml:space="preserve">FINDWORDANDCLICK</t>
   </si>
   <si>
-    <t xml:space="preserve">REMOTEDESKTOPNSO,NSO</t>
+    <t xml:space="preserve">NSO,NSO</t>
   </si>
   <si>
     <t xml:space="preserve">REMOTEDESKTOPNSO,SENTRA</t>
@@ -111,7 +114,16 @@
     <t xml:space="preserve">1 </t>
   </si>
   <si>
-    <t xml:space="preserve">REMOTEDESKTOPNSO,Aceptar</t>
+    <t xml:space="preserve">FINDIAMGEANDCREATEAREGION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMOTEDESKTOPNSO,Aceptar_sentra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLICKINREGION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aceptar_sentra,Aceptar_sentra</t>
   </si>
 </sst>
 </file>
@@ -169,8 +181,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -244,7 +257,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -325,15 +338,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.69"/>
   </cols>
   <sheetData>
@@ -420,7 +433,7 @@
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -466,34 +479,34 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,28 +514,28 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>19</v>
@@ -532,7 +545,7 @@
       <c r="B26" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -540,36 +553,58 @@
       <c r="B27" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="0"/>
+      <c r="B28" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>20</v>
+      <c r="C30" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>